<commit_message>
update bug report OLX
</commit_message>
<xml_diff>
--- a/olx/BugReport OLX.xlsx
+++ b/olx/BugReport OLX.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dima\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dima\Documents\github bugs\My-BugReports\olx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,45 +25,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Предварительное условие:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>URL: https://www.olx.ua</t>
   </si>
   <si>
-    <t>Шаги воспроизведения:</t>
-  </si>
-  <si>
     <t>1. Кликнуть на "Мой профиль".</t>
   </si>
   <si>
     <t xml:space="preserve">2. Для изменеия языка на сайте вверху на ленте кликнуть на "мова". </t>
   </si>
   <si>
-    <t>Все страница отображается переведена на украинский язык.</t>
-  </si>
-  <si>
-    <t>Ожидаемый результат:</t>
-  </si>
-  <si>
-    <t>Фактический результат:</t>
-  </si>
-  <si>
-    <t>Слово "текущий" переведено на слово "поточный" с буквой "ы".</t>
-  </si>
-  <si>
-    <t>Открывается страница для регистрации</t>
-  </si>
-  <si>
-    <t>Заглавие</t>
-  </si>
-  <si>
-    <t>Не верно переведено слово "Текущий" Отображается слово "поточный" с буквой "ы".</t>
-  </si>
-  <si>
-    <t>TC 1</t>
+    <t>Test Designed date:</t>
+  </si>
+  <si>
+    <t>Test Executed by:</t>
+  </si>
+  <si>
+    <t>Test Executed date:</t>
+  </si>
+  <si>
+    <t>Module name: Registration of a new customer</t>
+  </si>
+  <si>
+    <t>Test Priority:</t>
+  </si>
+  <si>
+    <t>Tesk?AC ID: TC1</t>
+  </si>
+  <si>
+    <t>Test Title: Registration of a new customer with valid data</t>
+  </si>
+  <si>
+    <t>Description:</t>
+  </si>
+  <si>
+    <t>Pre-conditions:</t>
+  </si>
+  <si>
+    <t>Data for testing:  Vasya Pupkin@gmail.com</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Enwiroment: Windows 10, Chrome</t>
+  </si>
+  <si>
+    <t>Test Designed by: Lutsenko D.</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>The word "Текущий" is not translated correctly. The word "streaming" with the letter "ы" is displayed.</t>
+  </si>
+  <si>
+    <t>The registration page opens. The entire page is displayed translated into Ukrainian.</t>
   </si>
 </sst>
 </file>
@@ -100,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -118,10 +139,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,66 +444,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A1:A6"/>
+  <mergeCells count="3">
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>